<commit_message>
Actual results of manual testcases
</commit_message>
<xml_diff>
--- a/Admin/Invoices/Manual testcases/Processed invoice.xlsx
+++ b/Admin/Invoices/Manual testcases/Processed invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Admin\Invoices\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584AD222-FA8D-4871-B526-0DF942A0CD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE0EF2F-2F4D-49E5-8409-CAFB20D51928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>SL. No</t>
   </si>
@@ -224,12 +224,36 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (new)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Once select the invoices digitizing page  we can edit the quickly open </t>
+      <t xml:space="preserve"> (new) &gt; Edit</t>
+    </r>
+  </si>
+  <si>
+    <t>Its gets displayed the Open Market list and Open catalogue page and click the Refresh market list data then will get the result</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Once select the invoices digitizing page  we can edit the quickly </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Open</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -651,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +818,13 @@
         <v>23</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>24</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>